<commit_message>
feat Backend : Group - Add Group Name on the template and modify Upload Endpoint
</commit_message>
<xml_diff>
--- a/Backend/Templates/GroupMembersTemplate.xlsx
+++ b/Backend/Templates/GroupMembersTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verio\Documents\Work\fork\SBMLiterationApp\Backend\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7173AA-30E5-448E-8B61-D7AA2365233B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924FF80-F6FE-468B-89D2-ECABF997CF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2904" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>NIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group Name </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,6 +48,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -92,11 +103,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,17 +389,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="1" max="2" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>